<commit_message>
feat(runners): send consolidated email in parallel PS1; remove duplicate email from batch wrappers
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-23.xlsx
+++ b/WB_Test_Report_2025-12-23.xlsx
@@ -9,11 +9,6 @@
     <sheet name="BOP_3" sheetId="4" r:id="rId4"/>
     <sheet name="BOP_4" sheetId="5" r:id="rId5"/>
     <sheet name="BOP_5" sheetId="6" r:id="rId6"/>
-    <sheet name="Package_1" sheetId="7" r:id="rId7"/>
-    <sheet name="Package_2" sheetId="8" r:id="rId8"/>
-    <sheet name="Package_3" sheetId="9" r:id="rId9"/>
-    <sheet name="Package_4" sheetId="10" r:id="rId10"/>
-    <sheet name="Package_5" sheetId="11" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
@@ -407,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -440,22 +435,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP (WI)</v>
+        <v>BOP (DE)</v>
       </c>
       <c r="C2" t="str">
-        <v>N/A</v>
+        <v>3003179466</v>
       </c>
       <c r="D2" t="str">
-        <v>N/A</v>
+        <v>1003052748</v>
       </c>
       <c r="E2" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="F2" t="str">
-        <v>72.94</v>
+        <v>471.73</v>
       </c>
       <c r="G2" t="str">
-        <v>WI</v>
+        <v>DE</v>
       </c>
     </row>
     <row r="3">
@@ -463,22 +458,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>BOP (DE)</v>
+        <v>BOP (MI)</v>
       </c>
       <c r="C3" t="str">
-        <v>N/A</v>
+        <v>3003179468</v>
       </c>
       <c r="D3" t="str">
-        <v>N/A</v>
+        <v>1003052749</v>
       </c>
       <c r="E3" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="F3" t="str">
-        <v>82.99</v>
+        <v>474.58</v>
       </c>
       <c r="G3" t="str">
-        <v>DE</v>
+        <v>MI</v>
       </c>
     </row>
     <row r="4">
@@ -486,22 +481,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>BOP (PA)</v>
+        <v>BOP (OH)</v>
       </c>
       <c r="C4" t="str">
-        <v>N/A</v>
+        <v>3003179467</v>
       </c>
       <c r="D4" t="str">
-        <v>N/A</v>
+        <v>1003052750</v>
       </c>
       <c r="E4" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="F4" t="str">
-        <v>83.31</v>
+        <v>472.87</v>
       </c>
       <c r="G4" t="str">
-        <v>PA</v>
+        <v>OH</v>
       </c>
     </row>
     <row r="5">
@@ -509,7 +504,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>BOP (OH)</v>
+        <v>BOP (WI)</v>
       </c>
       <c r="C5" t="str">
         <v>N/A</v>
@@ -521,10 +516,10 @@
         <v>FAILED</v>
       </c>
       <c r="F5" t="str">
-        <v>81.88</v>
+        <v>229.60</v>
       </c>
       <c r="G5" t="str">
-        <v>OH</v>
+        <v>WI</v>
       </c>
     </row>
     <row r="6">
@@ -532,149 +527,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>BOP (OH)</v>
+        <v>BOP (PA)</v>
       </c>
       <c r="C6" t="str">
-        <v>N/A</v>
+        <v>3003179473</v>
       </c>
       <c r="D6" t="str">
-        <v>N/A</v>
+        <v>1003052752</v>
       </c>
       <c r="E6" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="F6" t="str">
-        <v>81.88</v>
+        <v>461.65</v>
       </c>
       <c r="G6" t="str">
-        <v>OH</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Package (DE)</v>
-      </c>
-      <c r="C7" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D7" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E7" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="F7" t="str">
-        <v>73.20</v>
-      </c>
-      <c r="G7" t="str">
-        <v>DE</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Package (WI)</v>
-      </c>
-      <c r="C8" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D8" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E8" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="F8" t="str">
-        <v>72.96</v>
-      </c>
-      <c r="G8" t="str">
-        <v>WI</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Package (PA)</v>
-      </c>
-      <c r="C9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E9" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="F9" t="str">
-        <v>82.39</v>
-      </c>
-      <c r="G9" t="str">
         <v>PA</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Package (MI)</v>
-      </c>
-      <c r="C10" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D10" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E10" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="F10" t="str">
-        <v>70.81</v>
-      </c>
-      <c r="G10" t="str">
-        <v>MI</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Package (OH)</v>
-      </c>
-      <c r="C11" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D11" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E11" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="F11" t="str">
-        <v>81.17</v>
-      </c>
-      <c r="G11" t="str">
-        <v>OH</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -695,28 +575,98 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Test Execution Failed</v>
+        <v>Account Created</v>
       </c>
       <c r="B2" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>70.81s</v>
+        <v>87.36s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-23T15:12:40.840Z</v>
+        <v>2025-12-23T20:33:39.566Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>126.43s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-23T20:35:46.003Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>21.35s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-23T20:36:07.358Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>33.52s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-23T20:36:40.886Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>55.00s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-23T20:37:35.891Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>148.07s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-23T20:40:03.967Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -737,28 +687,98 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Test Execution Failed</v>
+        <v>Account Created</v>
       </c>
       <c r="B2" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>81.17s</v>
+        <v>91.27s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-23T15:12:50.490Z</v>
+        <v>2025-12-23T20:33:43.251Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>128.61s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-23T20:35:51.861Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>22.82s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-23T20:36:14.680Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>36.95s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-23T20:36:51.633Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>46.11s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-23T20:37:37.744Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>148.82s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-23T20:40:06.569Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -779,28 +799,98 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Test Execution Failed</v>
+        <v>Account Created</v>
       </c>
       <c r="B2" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>72.94s</v>
+        <v>85.67s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-23T15:08:00.494Z</v>
+        <v>2025-12-23T20:33:42.761Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>135.38s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-23T20:35:58.141Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>24.55s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-23T20:36:22.688Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>35.85s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-23T20:36:58.545Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>40.56s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-23T20:37:39.103Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>150.86s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-23T20:40:09.966Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -821,28 +911,42 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>84.12s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-23T20:41:39.823Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>Test Execution Failed</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <v>FAILED</v>
       </c>
-      <c r="C2" t="str">
-        <v>82.99s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-23T15:08:06.801Z</v>
+      <c r="C3" t="str">
+        <v>145.48s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-23T20:44:05.307Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -863,231 +967,91 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Test Execution Failed</v>
+        <v>Account Created</v>
       </c>
       <c r="B2" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>83.31s</v>
+        <v>83.33s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-23T15:08:07.612Z</v>
+        <v>2025-12-23T20:41:38.214Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>132.96s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-23T20:43:51.180Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>18.96s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-23T20:44:10.138Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>36.57s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-23T20:44:46.710Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>40.66s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-23T20:45:27.370Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>149.17s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-23T20:47:56.540Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>81.88s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-23T15:09:34.267Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>81.88s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-23T15:09:34.267Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>73.20s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-23T15:11:15.347Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>72.96s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-23T15:11:19.005Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>82.39s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-23T15:11:25.313Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>